<commit_message>
added rev 1 final fab files
</commit_message>
<xml_diff>
--- a/AHC-20-001_DP_Switch_Barrier_Block_Interface/AHC-20-001_DP_Switch_Barrier_Block_Interface_bom.xlsx
+++ b/AHC-20-001_DP_Switch_Barrier_Block_Interface/AHC-20-001_DP_Switch_Barrier_Block_Interface_bom.xlsx
@@ -95,7 +95,7 @@
     <t>PSF102-7651-711</t>
   </si>
   <si>
-    <t>J5 J6</t>
+    <t>TP1 TP2 TP3 TP4</t>
   </si>
   <si>
     <t>DNI</t>
@@ -420,15 +420,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
rev c files final
</commit_message>
<xml_diff>
--- a/AHC-20-001_DP_Switch_Barrier_Block_Interface/AHC-20-001_DP_Switch_Barrier_Block_Interface_bom.xlsx
+++ b/AHC-20-001_DP_Switch_Barrier_Block_Interface/AHC-20-001_DP_Switch_Barrier_Block_Interface_bom.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
   <si>
     <t>Item Number</t>
   </si>
@@ -95,10 +95,22 @@
     <t>PSF102-7651-711</t>
   </si>
   <si>
-    <t>TP1 TP2 TP3 TP4</t>
-  </si>
-  <si>
-    <t>DNI</t>
+    <t>J5 J6</t>
+  </si>
+  <si>
+    <t>JST Sales America Inc.</t>
+  </si>
+  <si>
+    <t>B2B-XH-AM(LF)(SN)</t>
+  </si>
+  <si>
+    <t>1x2pin 100mil</t>
+  </si>
+  <si>
+    <t>250V</t>
+  </si>
+  <si>
+    <t>CONN HEADER VERT 2POS 2.5MM</t>
   </si>
 </sst>
 </file>
@@ -426,11 +438,11 @@
   <cols>
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="31.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -556,7 +568,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>23</v>
@@ -565,19 +577,19 @@
         <v>24</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added REV D files
</commit_message>
<xml_diff>
--- a/AHC-20-001_DP_Switch_Barrier_Block_Interface/AHC-20-001_DP_Switch_Barrier_Block_Interface_bom.xlsx
+++ b/AHC-20-001_DP_Switch_Barrier_Block_Interface/AHC-20-001_DP_Switch_Barrier_Block_Interface_bom.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
   <si>
     <t>Item Number</t>
   </si>
@@ -111,6 +111,21 @@
   </si>
   <si>
     <t>CONN HEADER VERT 2POS 2.5MM</t>
+  </si>
+  <si>
+    <t>J7 J8 J9 J10</t>
+  </si>
+  <si>
+    <t>Essentra Components</t>
+  </si>
+  <si>
+    <t>LCBSB-4-01A-RT</t>
+  </si>
+  <si>
+    <t>700mil Square</t>
+  </si>
+  <si>
+    <t>BRD SPT SNAP LOCK ADHESIVE 1/4"</t>
   </si>
 </sst>
 </file>
@@ -430,21 +445,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -592,6 +609,35 @@
         <v>28</v>
       </c>
     </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>